<commit_message>
update figures after consistent convention fix
</commit_message>
<xml_diff>
--- a/runtime.xlsx
+++ b/runtime.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="396">
   <si>
     <t>\# \glspl{gb}</t>
   </si>
@@ -805,6 +805,402 @@
   </si>
   <si>
     <t>$3.702 \pm 0.8103$</t>
+  </si>
+  <si>
+    <t>\gls{vfzo} Set Size</t>
+  </si>
+  <si>
+    <t>\num{100}</t>
+  </si>
+  <si>
+    <t>\num{388}</t>
+  </si>
+  <si>
+    <t>\num{500}</t>
+  </si>
+  <si>
+    <t>\num{1000}</t>
+  </si>
+  <si>
+    <t>\num{5000}</t>
+  </si>
+  <si>
+    <t>\num{10000}</t>
+  </si>
+  <si>
+    <t>\num{20000}</t>
+  </si>
+  <si>
+    <t>\num{50000}</t>
+  </si>
+  <si>
+    <t>Barycentric</t>
+  </si>
+  <si>
+    <t>$201.7 \pm 23.32$</t>
+  </si>
+  <si>
+    <t>$446.7 \pm 40.35$</t>
+  </si>
+  <si>
+    <t>$446.3 \pm 23.66$</t>
+  </si>
+  <si>
+    <t>$585.9 \pm 72.3$</t>
+  </si>
+  <si>
+    <t>$1003 \pm 58.16$</t>
+  </si>
+  <si>
+    <t>$1532 \pm 48.24$</t>
+  </si>
+  <si>
+    <t>$2576 \pm 225.4$</t>
+  </si>
+  <si>
+    <t>$5974 \pm 409.3$</t>
+  </si>
+  <si>
+    <t>GPR</t>
+  </si>
+  <si>
+    <t>IDW</t>
+  </si>
+  <si>
+    <t>NN</t>
+  </si>
+  <si>
+    <t>\gls{vfzo} Set Size</t>
+  </si>
+  <si>
+    <t>\num{100}</t>
+  </si>
+  <si>
+    <t>\num{388}</t>
+  </si>
+  <si>
+    <t>\num{500}</t>
+  </si>
+  <si>
+    <t>\num{1000}</t>
+  </si>
+  <si>
+    <t>\num{5000}</t>
+  </si>
+  <si>
+    <t>\num{10000}</t>
+  </si>
+  <si>
+    <t>\num{20000}</t>
+  </si>
+  <si>
+    <t>\num{50000}</t>
+  </si>
+  <si>
+    <t>Barycentric</t>
+  </si>
+  <si>
+    <t>$201.7 \pm 23.32$</t>
+  </si>
+  <si>
+    <t>$446.7 \pm 40.35$</t>
+  </si>
+  <si>
+    <t>$446.3 \pm 23.66$</t>
+  </si>
+  <si>
+    <t>$585.9 \pm 72.3$</t>
+  </si>
+  <si>
+    <t>$1003 \pm 58.16$</t>
+  </si>
+  <si>
+    <t>$1532 \pm 48.24$</t>
+  </si>
+  <si>
+    <t>$2576 \pm 225.4$</t>
+  </si>
+  <si>
+    <t>$5974 \pm 409.3$</t>
+  </si>
+  <si>
+    <t>GPR</t>
+  </si>
+  <si>
+    <t>$0.449 \pm 0.3267$</t>
+  </si>
+  <si>
+    <t>$0.785 \pm 0.3499$</t>
+  </si>
+  <si>
+    <t>$0.7522 \pm 0.3859$</t>
+  </si>
+  <si>
+    <t>$1.969 \pm 0.5057$</t>
+  </si>
+  <si>
+    <t>$5.665 \pm 0.8914$</t>
+  </si>
+  <si>
+    <t>$7.555 \pm 3.305$</t>
+  </si>
+  <si>
+    <t>$10.95 \pm 3.454$</t>
+  </si>
+  <si>
+    <t>$16.06 \pm 5.49$</t>
+  </si>
+  <si>
+    <t>IDW</t>
+  </si>
+  <si>
+    <t>NN</t>
+  </si>
+  <si>
+    <t>\gls{vfzo} Set Size</t>
+  </si>
+  <si>
+    <t>\num{100}</t>
+  </si>
+  <si>
+    <t>\num{388}</t>
+  </si>
+  <si>
+    <t>\num{500}</t>
+  </si>
+  <si>
+    <t>\num{1000}</t>
+  </si>
+  <si>
+    <t>\num{5000}</t>
+  </si>
+  <si>
+    <t>\num{10000}</t>
+  </si>
+  <si>
+    <t>\num{20000}</t>
+  </si>
+  <si>
+    <t>\num{50000}</t>
+  </si>
+  <si>
+    <t>Barycentric</t>
+  </si>
+  <si>
+    <t>$201.7 \pm 23.32$</t>
+  </si>
+  <si>
+    <t>$446.7 \pm 40.35$</t>
+  </si>
+  <si>
+    <t>$446.3 \pm 23.66$</t>
+  </si>
+  <si>
+    <t>$585.9 \pm 72.3$</t>
+  </si>
+  <si>
+    <t>$1003 \pm 58.16$</t>
+  </si>
+  <si>
+    <t>$1532 \pm 48.24$</t>
+  </si>
+  <si>
+    <t>$2576 \pm 225.4$</t>
+  </si>
+  <si>
+    <t>$5974 \pm 409.3$</t>
+  </si>
+  <si>
+    <t>GPR</t>
+  </si>
+  <si>
+    <t>$0.449 \pm 0.3267$</t>
+  </si>
+  <si>
+    <t>$0.785 \pm 0.3499$</t>
+  </si>
+  <si>
+    <t>$0.7522 \pm 0.3859$</t>
+  </si>
+  <si>
+    <t>$1.969 \pm 0.5057$</t>
+  </si>
+  <si>
+    <t>$5.665 \pm 0.8914$</t>
+  </si>
+  <si>
+    <t>$7.555 \pm 3.305$</t>
+  </si>
+  <si>
+    <t>$10.95 \pm 3.454$</t>
+  </si>
+  <si>
+    <t>$16.06 \pm 5.49$</t>
+  </si>
+  <si>
+    <t>IDW</t>
+  </si>
+  <si>
+    <t>$0.0387 \pm 0.0112$</t>
+  </si>
+  <si>
+    <t>$0.1012 \pm 0.0198$</t>
+  </si>
+  <si>
+    <t>$0.1168 \pm 0.0252$</t>
+  </si>
+  <si>
+    <t>$0.1842 \pm 0.021$</t>
+  </si>
+  <si>
+    <t>$0.8725 \pm 0.1618$</t>
+  </si>
+  <si>
+    <t>$1.436 \pm 0.3621$</t>
+  </si>
+  <si>
+    <t>$3.396 \pm 0.8363$</t>
+  </si>
+  <si>
+    <t>$6.759 \pm 1.244$</t>
+  </si>
+  <si>
+    <t>NN</t>
+  </si>
+  <si>
+    <t>\gls{vfzo} Set Size</t>
+  </si>
+  <si>
+    <t>\num{100}</t>
+  </si>
+  <si>
+    <t>\num{388}</t>
+  </si>
+  <si>
+    <t>\num{500}</t>
+  </si>
+  <si>
+    <t>\num{1000}</t>
+  </si>
+  <si>
+    <t>\num{5000}</t>
+  </si>
+  <si>
+    <t>\num{10000}</t>
+  </si>
+  <si>
+    <t>\num{20000}</t>
+  </si>
+  <si>
+    <t>\num{50000}</t>
+  </si>
+  <si>
+    <t>Barycentric</t>
+  </si>
+  <si>
+    <t>$201.7 \pm 23.32$</t>
+  </si>
+  <si>
+    <t>$446.7 \pm 40.35$</t>
+  </si>
+  <si>
+    <t>$446.3 \pm 23.66$</t>
+  </si>
+  <si>
+    <t>$585.9 \pm 72.3$</t>
+  </si>
+  <si>
+    <t>$1003 \pm 58.16$</t>
+  </si>
+  <si>
+    <t>$1532 \pm 48.24$</t>
+  </si>
+  <si>
+    <t>$2576 \pm 225.4$</t>
+  </si>
+  <si>
+    <t>$5974 \pm 409.3$</t>
+  </si>
+  <si>
+    <t>GPR</t>
+  </si>
+  <si>
+    <t>$0.449 \pm 0.3267$</t>
+  </si>
+  <si>
+    <t>$0.785 \pm 0.3499$</t>
+  </si>
+  <si>
+    <t>$0.7522 \pm 0.3859$</t>
+  </si>
+  <si>
+    <t>$1.969 \pm 0.5057$</t>
+  </si>
+  <si>
+    <t>$5.665 \pm 0.8914$</t>
+  </si>
+  <si>
+    <t>$7.555 \pm 3.305$</t>
+  </si>
+  <si>
+    <t>$10.95 \pm 3.454$</t>
+  </si>
+  <si>
+    <t>$16.06 \pm 5.49$</t>
+  </si>
+  <si>
+    <t>IDW</t>
+  </si>
+  <si>
+    <t>$0.0387 \pm 0.0112$</t>
+  </si>
+  <si>
+    <t>$0.1012 \pm 0.0198$</t>
+  </si>
+  <si>
+    <t>$0.1168 \pm 0.0252$</t>
+  </si>
+  <si>
+    <t>$0.1842 \pm 0.021$</t>
+  </si>
+  <si>
+    <t>$0.8725 \pm 0.1618$</t>
+  </si>
+  <si>
+    <t>$1.436 \pm 0.3621$</t>
+  </si>
+  <si>
+    <t>$3.396 \pm 0.8363$</t>
+  </si>
+  <si>
+    <t>$6.759 \pm 1.244$</t>
+  </si>
+  <si>
+    <t>NN</t>
+  </si>
+  <si>
+    <t>$0.0417 \pm 0.0135$</t>
+  </si>
+  <si>
+    <t>$0.0954 \pm 0.0554$</t>
+  </si>
+  <si>
+    <t>$0.0922 \pm 0.0493$</t>
+  </si>
+  <si>
+    <t>$0.1946 \pm 0.1177$</t>
+  </si>
+  <si>
+    <t>$0.9267 \pm 0.2889$</t>
+  </si>
+  <si>
+    <t>$0.9959 \pm 0.1711$</t>
+  </si>
+  <si>
+    <t>$1.584 \pm 0.5634$</t>
+  </si>
+  <si>
+    <t>$2.91 \pm 1.054$</t>
   </si>
 </sst>
 </file>
@@ -825,7 +1221,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -841,11 +1237,15 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -855,6 +1255,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -876,155 +1280,155 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>219</v>
+        <v>351</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>228</v>
+        <v>360</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>237</v>
+        <v>369</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>246</v>
+        <v>378</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>255</v>
+        <v>387</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>220</v>
+        <v>352</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>229</v>
+        <v>361</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>238</v>
+        <v>370</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>247</v>
+        <v>379</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>256</v>
+        <v>388</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>221</v>
+        <v>353</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>230</v>
+        <v>362</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>239</v>
+        <v>371</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>248</v>
+        <v>380</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>257</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>222</v>
+        <v>354</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>231</v>
+        <v>363</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>240</v>
+        <v>372</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>249</v>
+        <v>381</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>258</v>
+        <v>390</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>223</v>
+        <v>355</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>232</v>
+        <v>364</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>241</v>
+        <v>373</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>250</v>
+        <v>382</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>259</v>
+        <v>391</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>224</v>
+        <v>356</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>233</v>
+        <v>365</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>242</v>
+        <v>374</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>251</v>
+        <v>383</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>260</v>
+        <v>392</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>225</v>
+        <v>357</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>234</v>
+        <v>366</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>243</v>
+        <v>375</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>252</v>
+        <v>384</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>261</v>
+        <v>393</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>226</v>
+        <v>358</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>235</v>
+        <v>367</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>244</v>
+        <v>376</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>253</v>
+        <v>385</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>262</v>
+        <v>394</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>227</v>
+        <v>359</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>236</v>
+        <v>368</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>245</v>
+        <v>377</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>254</v>
+        <v>386</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>263</v>
+        <v>395</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update figures/tables after proper spherical sampling
</commit_message>
<xml_diff>
--- a/runtime.xlsx
+++ b/runtime.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="528">
   <si>
     <t>\# \glspl{gb}</t>
   </si>
@@ -1201,6 +1201,402 @@
   </si>
   <si>
     <t>$2.91 \pm 1.054$</t>
+  </si>
+  <si>
+    <t>\gls{vfzo} Set Size</t>
+  </si>
+  <si>
+    <t>\num{100}</t>
+  </si>
+  <si>
+    <t>\num{388}</t>
+  </si>
+  <si>
+    <t>\num{500}</t>
+  </si>
+  <si>
+    <t>\num{1000}</t>
+  </si>
+  <si>
+    <t>\num{5000}</t>
+  </si>
+  <si>
+    <t>\num{10000}</t>
+  </si>
+  <si>
+    <t>\num{20000}</t>
+  </si>
+  <si>
+    <t>\num{50000}</t>
+  </si>
+  <si>
+    <t>Barycentric</t>
+  </si>
+  <si>
+    <t>$191.8 \pm 19.57$</t>
+  </si>
+  <si>
+    <t>$388.4 \pm 18.84$</t>
+  </si>
+  <si>
+    <t>$455.7 \pm 55.28$</t>
+  </si>
+  <si>
+    <t>$536.5 \pm 35.26$</t>
+  </si>
+  <si>
+    <t>$998.9 \pm 54.48$</t>
+  </si>
+  <si>
+    <t>$1516 \pm 56.59$</t>
+  </si>
+  <si>
+    <t>$2526 \pm 119.5$</t>
+  </si>
+  <si>
+    <t>$5743 \pm 361.3$</t>
+  </si>
+  <si>
+    <t>GPR</t>
+  </si>
+  <si>
+    <t>IDW</t>
+  </si>
+  <si>
+    <t>NN</t>
+  </si>
+  <si>
+    <t>\gls{vfzo} Set Size</t>
+  </si>
+  <si>
+    <t>\num{100}</t>
+  </si>
+  <si>
+    <t>\num{388}</t>
+  </si>
+  <si>
+    <t>\num{500}</t>
+  </si>
+  <si>
+    <t>\num{1000}</t>
+  </si>
+  <si>
+    <t>\num{5000}</t>
+  </si>
+  <si>
+    <t>\num{10000}</t>
+  </si>
+  <si>
+    <t>\num{20000}</t>
+  </si>
+  <si>
+    <t>\num{50000}</t>
+  </si>
+  <si>
+    <t>Barycentric</t>
+  </si>
+  <si>
+    <t>$191.8 \pm 19.57$</t>
+  </si>
+  <si>
+    <t>$388.4 \pm 18.84$</t>
+  </si>
+  <si>
+    <t>$455.7 \pm 55.28$</t>
+  </si>
+  <si>
+    <t>$536.5 \pm 35.26$</t>
+  </si>
+  <si>
+    <t>$998.9 \pm 54.48$</t>
+  </si>
+  <si>
+    <t>$1516 \pm 56.59$</t>
+  </si>
+  <si>
+    <t>$2526 \pm 119.5$</t>
+  </si>
+  <si>
+    <t>$5743 \pm 361.3$</t>
+  </si>
+  <si>
+    <t>GPR</t>
+  </si>
+  <si>
+    <t>$0.4187 \pm 0.4342$</t>
+  </si>
+  <si>
+    <t>$0.943 \pm 0.3481$</t>
+  </si>
+  <si>
+    <t>$0.6104 \pm 0.3138$</t>
+  </si>
+  <si>
+    <t>$1.743 \pm 0.9464$</t>
+  </si>
+  <si>
+    <t>$5.216 \pm 0.4816$</t>
+  </si>
+  <si>
+    <t>$5.609 \pm 0.8756$</t>
+  </si>
+  <si>
+    <t>$11.45 \pm 3.29$</t>
+  </si>
+  <si>
+    <t>$13.69 \pm 4.05$</t>
+  </si>
+  <si>
+    <t>IDW</t>
+  </si>
+  <si>
+    <t>NN</t>
+  </si>
+  <si>
+    <t>\gls{vfzo} Set Size</t>
+  </si>
+  <si>
+    <t>\num{100}</t>
+  </si>
+  <si>
+    <t>\num{388}</t>
+  </si>
+  <si>
+    <t>\num{500}</t>
+  </si>
+  <si>
+    <t>\num{1000}</t>
+  </si>
+  <si>
+    <t>\num{5000}</t>
+  </si>
+  <si>
+    <t>\num{10000}</t>
+  </si>
+  <si>
+    <t>\num{20000}</t>
+  </si>
+  <si>
+    <t>\num{50000}</t>
+  </si>
+  <si>
+    <t>Barycentric</t>
+  </si>
+  <si>
+    <t>$191.8 \pm 19.57$</t>
+  </si>
+  <si>
+    <t>$388.4 \pm 18.84$</t>
+  </si>
+  <si>
+    <t>$455.7 \pm 55.28$</t>
+  </si>
+  <si>
+    <t>$536.5 \pm 35.26$</t>
+  </si>
+  <si>
+    <t>$998.9 \pm 54.48$</t>
+  </si>
+  <si>
+    <t>$1516 \pm 56.59$</t>
+  </si>
+  <si>
+    <t>$2526 \pm 119.5$</t>
+  </si>
+  <si>
+    <t>$5743 \pm 361.3$</t>
+  </si>
+  <si>
+    <t>GPR</t>
+  </si>
+  <si>
+    <t>$0.4187 \pm 0.4342$</t>
+  </si>
+  <si>
+    <t>$0.943 \pm 0.3481$</t>
+  </si>
+  <si>
+    <t>$0.6104 \pm 0.3138$</t>
+  </si>
+  <si>
+    <t>$1.743 \pm 0.9464$</t>
+  </si>
+  <si>
+    <t>$5.216 \pm 0.4816$</t>
+  </si>
+  <si>
+    <t>$5.609 \pm 0.8756$</t>
+  </si>
+  <si>
+    <t>$11.45 \pm 3.29$</t>
+  </si>
+  <si>
+    <t>$13.69 \pm 4.05$</t>
+  </si>
+  <si>
+    <t>IDW</t>
+  </si>
+  <si>
+    <t>$0.034 \pm 0$</t>
+  </si>
+  <si>
+    <t>$0.0904 \pm 0.0224$</t>
+  </si>
+  <si>
+    <t>$0.1352 \pm 0.0364$</t>
+  </si>
+  <si>
+    <t>$0.1948 \pm 0.0395$</t>
+  </si>
+  <si>
+    <t>$0.8726 \pm 0.1529$</t>
+  </si>
+  <si>
+    <t>$1.631 \pm 0.3915$</t>
+  </si>
+  <si>
+    <t>$3.191 \pm 0.4752$</t>
+  </si>
+  <si>
+    <t>$7.635 \pm 1.872$</t>
+  </si>
+  <si>
+    <t>NN</t>
+  </si>
+  <si>
+    <t>\gls{vfzo} Set Size</t>
+  </si>
+  <si>
+    <t>\num{100}</t>
+  </si>
+  <si>
+    <t>\num{388}</t>
+  </si>
+  <si>
+    <t>\num{500}</t>
+  </si>
+  <si>
+    <t>\num{1000}</t>
+  </si>
+  <si>
+    <t>\num{5000}</t>
+  </si>
+  <si>
+    <t>\num{10000}</t>
+  </si>
+  <si>
+    <t>\num{20000}</t>
+  </si>
+  <si>
+    <t>\num{50000}</t>
+  </si>
+  <si>
+    <t>Barycentric</t>
+  </si>
+  <si>
+    <t>$191.8 \pm 19.57$</t>
+  </si>
+  <si>
+    <t>$388.4 \pm 18.84$</t>
+  </si>
+  <si>
+    <t>$455.7 \pm 55.28$</t>
+  </si>
+  <si>
+    <t>$536.5 \pm 35.26$</t>
+  </si>
+  <si>
+    <t>$998.9 \pm 54.48$</t>
+  </si>
+  <si>
+    <t>$1516 \pm 56.59$</t>
+  </si>
+  <si>
+    <t>$2526 \pm 119.5$</t>
+  </si>
+  <si>
+    <t>$5743 \pm 361.3$</t>
+  </si>
+  <si>
+    <t>GPR</t>
+  </si>
+  <si>
+    <t>$0.4187 \pm 0.4342$</t>
+  </si>
+  <si>
+    <t>$0.943 \pm 0.3481$</t>
+  </si>
+  <si>
+    <t>$0.6104 \pm 0.3138$</t>
+  </si>
+  <si>
+    <t>$1.743 \pm 0.9464$</t>
+  </si>
+  <si>
+    <t>$5.216 \pm 0.4816$</t>
+  </si>
+  <si>
+    <t>$5.609 \pm 0.8756$</t>
+  </si>
+  <si>
+    <t>$11.45 \pm 3.29$</t>
+  </si>
+  <si>
+    <t>$13.69 \pm 4.05$</t>
+  </si>
+  <si>
+    <t>IDW</t>
+  </si>
+  <si>
+    <t>$0.034 \pm 0$</t>
+  </si>
+  <si>
+    <t>$0.0904 \pm 0.0224$</t>
+  </si>
+  <si>
+    <t>$0.1352 \pm 0.0364$</t>
+  </si>
+  <si>
+    <t>$0.1948 \pm 0.0395$</t>
+  </si>
+  <si>
+    <t>$0.8726 \pm 0.1529$</t>
+  </si>
+  <si>
+    <t>$1.631 \pm 0.3915$</t>
+  </si>
+  <si>
+    <t>$3.191 \pm 0.4752$</t>
+  </si>
+  <si>
+    <t>$7.635 \pm 1.872$</t>
+  </si>
+  <si>
+    <t>NN</t>
+  </si>
+  <si>
+    <t>$0.0367 \pm 0.0041$</t>
+  </si>
+  <si>
+    <t>$0.0705 \pm 0.0129$</t>
+  </si>
+  <si>
+    <t>$0.0724 \pm 0.0051$</t>
+  </si>
+  <si>
+    <t>$0.1203 \pm 0.0184$</t>
+  </si>
+  <si>
+    <t>$0.9277 \pm 0.2418$</t>
+  </si>
+  <si>
+    <t>$0.8938 \pm 0.1717$</t>
+  </si>
+  <si>
+    <t>$1.275 \pm 0.3423$</t>
+  </si>
+  <si>
+    <t>$3.817 \pm 0.5884$</t>
   </si>
 </sst>
 </file>
@@ -1221,7 +1617,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1241,11 +1637,15 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -1259,6 +1659,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1280,155 +1684,155 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>351</v>
+        <v>483</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>360</v>
+        <v>492</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>369</v>
+        <v>501</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>378</v>
+        <v>510</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>387</v>
+        <v>519</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>352</v>
+        <v>484</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>361</v>
+        <v>493</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>370</v>
+        <v>502</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>379</v>
+        <v>511</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>388</v>
+        <v>520</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>353</v>
+        <v>485</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>362</v>
+        <v>494</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>371</v>
+        <v>503</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>380</v>
+        <v>512</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>389</v>
+        <v>521</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>354</v>
+        <v>486</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>363</v>
+        <v>495</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>372</v>
+        <v>504</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>381</v>
+        <v>513</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>390</v>
+        <v>522</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>355</v>
+        <v>487</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>364</v>
+        <v>496</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>373</v>
+        <v>505</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>382</v>
+        <v>514</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>391</v>
+        <v>523</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>356</v>
+        <v>488</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>365</v>
+        <v>497</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>374</v>
+        <v>506</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>383</v>
+        <v>515</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>392</v>
+        <v>524</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>357</v>
+        <v>489</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>366</v>
+        <v>498</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>375</v>
+        <v>507</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>384</v>
+        <v>516</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>393</v>
+        <v>525</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>358</v>
+        <v>490</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>367</v>
+        <v>499</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>376</v>
+        <v>508</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>385</v>
+        <v>517</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>394</v>
+        <v>526</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>359</v>
+        <v>491</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>368</v>
+        <v>500</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>377</v>
+        <v>509</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>386</v>
+        <v>518</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>395</v>
+        <v>527</v>
       </c>
     </row>
   </sheetData>

</xml_diff>